<commit_message>
update of analyses (apart from complementizers)
</commit_message>
<xml_diff>
--- a/data/excel/BrNews_deceive.xlsx
+++ b/data/excel/BrNews_deceive.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ba4es16\Work Folders\Documents\Aufsätze\Leuven 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ba4es16\Work Folders\Documents\Aufsätze\Leuven 2022\R_project_verbs_of_deceiving\data\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -926,11 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2:I173"/>
     </sheetView>
   </sheetViews>
@@ -1165,7 +1164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1357,7 +1356,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
@@ -1389,7 +1388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>9</v>
       </c>
@@ -1645,7 +1644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
@@ -1709,7 +1708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1837,7 +1836,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>9</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>9</v>
       </c>
@@ -1901,7 +1900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
@@ -1997,7 +1996,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>9</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>9</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>9</v>
       </c>
@@ -2093,7 +2092,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>9</v>
       </c>
@@ -3373,7 +3372,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>9</v>
       </c>
@@ -3405,7 +3404,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>9</v>
       </c>
@@ -3437,7 +3436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>9</v>
       </c>
@@ -3469,7 +3468,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>9</v>
       </c>
@@ -3501,7 +3500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>9</v>
       </c>
@@ -3693,7 +3692,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>9</v>
       </c>
@@ -3917,7 +3916,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>9</v>
       </c>
@@ -4173,7 +4172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>9</v>
       </c>
@@ -4333,7 +4332,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>9</v>
       </c>
@@ -4365,7 +4364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>9</v>
       </c>
@@ -4397,7 +4396,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>9</v>
       </c>
@@ -4429,7 +4428,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>9</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>9</v>
       </c>
@@ -4653,7 +4652,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>9</v>
       </c>
@@ -4685,7 +4684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>9</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>9</v>
       </c>
@@ -4749,7 +4748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>9</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>9</v>
       </c>
@@ -4813,7 +4812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>9</v>
       </c>
@@ -4845,7 +4844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>9</v>
       </c>
@@ -4909,7 +4908,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>9</v>
       </c>
@@ -4941,7 +4940,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>9</v>
       </c>
@@ -4973,7 +4972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>9</v>
       </c>
@@ -6253,7 +6252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="167" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>9</v>
       </c>
@@ -6285,7 +6284,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>9</v>
       </c>
@@ -6317,7 +6316,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>9</v>
       </c>
@@ -6349,7 +6348,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="170" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>9</v>
       </c>
@@ -6477,7 +6476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>9</v>
       </c>
@@ -6509,7 +6508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>9</v>
       </c>
@@ -6541,7 +6540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
         <v>9</v>
       </c>
@@ -6574,17 +6573,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J176">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="in believing"/>
-        <filter val="in thinking"/>
-        <filter val="into believing"/>
-        <filter val="into thinking"/>
-        <filter val="to think"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J176"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>